<commit_message>
Fix add record to add multiple records in session
</commit_message>
<xml_diff>
--- a/datasets/taxes2022.xlsx
+++ b/datasets/taxes2022.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,7 +511,9 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="n">
+        <v>7107</v>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>CP 1099</t>
@@ -519,7 +521,11 @@
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>wells fargo</t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -536,8 +542,12 @@
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>35803.4</v>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
           <t>Toyota W-2</t>
@@ -546,7 +556,63 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Wages, tips, other comp.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>16afe2b7-b1ee-4c6a-ad30-699637f33f6f</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>01/31/2023</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>tw22</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>b6818292-a689-4a17-8b0f-ea2f05de255a</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>01/31/2023</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>tw23</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>